<commit_message>
UPD data from 2020-05-10
</commit_message>
<xml_diff>
--- a/index_si_moscow_stpetersburg_sevastopol.xlsx
+++ b/index_si_moscow_stpetersburg_sevastopol.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="83">
   <si>
     <t>state</t>
   </si>
@@ -248,6 +248,12 @@
   </si>
   <si>
     <t>2020-05-07</t>
+  </si>
+  <si>
+    <t>2020-05-08</t>
+  </si>
+  <si>
+    <t>2020-05-09</t>
   </si>
   <si>
     <t>Севастополь</t>
@@ -633,7 +639,7 @@
   <sheetPr>
     <tabColor rgb="FFEBA00"/>
   </sheetPr>
-  <dimension ref="A1:C226"/>
+  <dimension ref="A1:C232"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
@@ -1478,54 +1484,54 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
+        <v>3</v>
+      </c>
+      <c r="B77" t="s">
         <v>79</v>
       </c>
-      <c r="B77" t="s">
-        <v>4</v>
-      </c>
       <c r="C77">
-        <v>3</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>79</v>
+        <v>3</v>
       </c>
       <c r="B78" t="s">
-        <v>5</v>
+        <v>80</v>
       </c>
       <c r="C78">
-        <v>3.4</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B79" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C79">
-        <v>1.6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B80" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C80">
-        <v>1.6</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B81" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C81">
         <v>1.6</v>
@@ -1533,87 +1539,87 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C82">
-        <v>1.7</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B83" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C83">
-        <v>2.6</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B84" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C84">
-        <v>3</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B85" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C85">
-        <v>1.7</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B86" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C86">
-        <v>1.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B87" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C87">
-        <v>1.4</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B88" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C88">
-        <v>1.4</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B89" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C89">
         <v>1.4</v>
@@ -1621,318 +1627,318 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B90" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C90">
-        <v>2.3</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B91" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C91">
-        <v>2.6</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B92" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C92">
-        <v>2.9</v>
+        <v>2.3</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B93" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C93">
-        <v>1.5</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B94" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C94">
-        <v>1.5</v>
+        <v>2.9</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B95" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C95">
-        <v>1.4</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B96" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C96">
-        <v>1.4</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B97" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C97">
-        <v>2.5</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B98" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C98">
-        <v>3.3</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B99" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C99">
-        <v>1.6</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B100" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C100">
-        <v>1.5</v>
+        <v>3.3</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B101" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C101">
-        <v>2.5</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B102" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C102">
-        <v>1.9</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B103" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C103">
-        <v>1.8</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B104" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C104">
-        <v>2.5</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B105" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C105">
-        <v>3.1</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B106" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C106">
-        <v>2.1</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B107" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C107">
-        <v>2</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B108" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C108">
-        <v>1.9</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B109" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C109">
-        <v>1.9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B110" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C110">
-        <v>2</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B111" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C111">
-        <v>3.1</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B112" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C112">
-        <v>3.7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B113" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C113">
-        <v>3.2</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B114" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C114">
-        <v>3.4</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B115" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C115">
-        <v>3.6</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B116" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C116">
-        <v>3.9</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B117" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C117">
-        <v>3.7</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B118" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C118">
         <v>3.9</v>
@@ -1940,175 +1946,175 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B119" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C119">
-        <v>4.1</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B120" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C120">
-        <v>3.5</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B121" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C121">
-        <v>3.4</v>
+        <v>4.1</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B122" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C122">
-        <v>3.3</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B123" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C123">
-        <v>3.3</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B124" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C124">
-        <v>3.2</v>
+        <v>3.3</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B125" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C125">
-        <v>3.5</v>
+        <v>3.3</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B126" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C126">
-        <v>3.9</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B127" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C127">
-        <v>3.2</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B128" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C128">
-        <v>3.1</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B129" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C129">
-        <v>3.3</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B130" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C130">
-        <v>3.2</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B131" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C131">
-        <v>3.1</v>
+        <v>3.3</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B132" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C132">
-        <v>3.5</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B133" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C133">
-        <v>3.8</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B134" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C134">
         <v>3.5</v>
@@ -2116,32 +2122,32 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B135" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C135">
-        <v>3</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B136" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C136">
-        <v>3</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B137" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C137">
         <v>3</v>
@@ -2149,120 +2155,120 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B138" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C138">
-        <v>2.9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B139" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C139">
-        <v>3.3</v>
+        <v>3</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B140" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C140">
-        <v>3.8</v>
+        <v>2.9</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B141" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C141">
-        <v>2.9</v>
+        <v>3.3</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B142" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C142">
-        <v>2.8</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B143" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C143">
-        <v>2.8</v>
+        <v>2.9</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B144" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C144">
-        <v>2.7</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B145" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C145">
-        <v>3.2</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B146" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C146">
-        <v>3.3</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B147" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C147">
-        <v>3.5</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B148" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C148">
         <v>3.3</v>
@@ -2270,219 +2276,219 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B149" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C149">
-        <v>3.2</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B150" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C150">
-        <v>2.7</v>
+        <v>3.3</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B151" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C151">
-        <v>2.7</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B152" t="s">
-        <v>4</v>
+        <v>77</v>
       </c>
       <c r="C152">
-        <v>2.5</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B153" t="s">
-        <v>5</v>
+        <v>78</v>
       </c>
       <c r="C153">
-        <v>2.6</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B154" t="s">
-        <v>6</v>
+        <v>79</v>
       </c>
       <c r="C154">
-        <v>0.4</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
+        <v>81</v>
+      </c>
+      <c r="B155" t="s">
         <v>80</v>
       </c>
-      <c r="B155" t="s">
-        <v>7</v>
-      </c>
       <c r="C155">
-        <v>0.4</v>
+        <v>3.3</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B156" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C156">
-        <v>0.4</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B157" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C157">
-        <v>0.5</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B158" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C158">
-        <v>2</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B159" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C159">
-        <v>2.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B160" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C160">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B161" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C161">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B162" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C162">
-        <v>0.4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B163" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C163">
-        <v>0.4</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B164" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C164">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B165" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C165">
-        <v>2</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B166" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C166">
-        <v>2.4</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B167" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C167">
-        <v>2.4</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B168" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C168">
         <v>0.4</v>
@@ -2490,384 +2496,384 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B169" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C169">
-        <v>0.4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B170" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C170">
-        <v>0.5</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B171" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C171">
-        <v>0.5</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B172" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C172">
-        <v>2.1</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B173" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C173">
-        <v>2.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B174" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C174">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B175" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C175">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B176" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C176">
-        <v>0.8</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B177" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C177">
-        <v>0.9</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B178" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C178">
-        <v>0.9</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B179" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C179">
-        <v>2.4</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B180" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C180">
-        <v>2.8</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B181" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C181">
-        <v>1</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B182" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C182">
-        <v>1.1</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B183" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C183">
-        <v>1</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B184" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C184">
-        <v>1.1</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B185" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C185">
-        <v>1.1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B186" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C186">
-        <v>3</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B187" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C187">
-        <v>3.6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B188" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C188">
-        <v>3</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B189" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C189">
-        <v>3.2</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B190" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C190">
-        <v>3.4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B191" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C191">
-        <v>3.5</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B192" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C192">
-        <v>3.4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B193" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C193">
-        <v>3.8</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B194" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C194">
-        <v>3.9</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B195" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C195">
-        <v>2.9</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B196" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C196">
-        <v>2.8</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B197" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C197">
-        <v>2.8</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B198" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C198">
-        <v>2.8</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B199" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C199">
-        <v>2.7</v>
+        <v>2.9</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B200" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C200">
-        <v>3.5</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B201" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C201">
-        <v>3.8</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B202" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C202">
-        <v>2.7</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B203" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C203">
         <v>2.7</v>
@@ -2875,32 +2881,32 @@
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B204" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C204">
-        <v>2.7</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B205" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C205">
-        <v>2.7</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B206" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C206">
         <v>2.7</v>
@@ -2908,32 +2914,32 @@
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B207" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C207">
-        <v>3.5</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B208" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C208">
-        <v>3.8</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B209" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C209">
         <v>2.7</v>
@@ -2941,76 +2947,76 @@
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B210" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C210">
-        <v>2.6</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B211" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C211">
-        <v>2.6</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B212" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C212">
-        <v>2.5</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B213" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C213">
-        <v>2.6</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B214" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C214">
-        <v>3.2</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B215" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C215">
-        <v>3.6</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B216" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C216">
         <v>2.5</v>
@@ -3018,112 +3024,178 @@
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B217" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C217">
-        <v>2.4</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B218" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C218">
-        <v>2.4</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B219" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C219">
-        <v>2.3</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B220" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C220">
-        <v>3.1</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B221" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C221">
-        <v>3.1</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B222" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C222">
-        <v>3.4</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B223" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C223">
-        <v>3</v>
+        <v>2.3</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B224" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C224">
-        <v>2.9</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B225" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C225">
-        <v>2.1</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
+        <v>82</v>
+      </c>
+      <c r="B226" t="s">
+        <v>74</v>
+      </c>
+      <c r="C226">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
+        <v>82</v>
+      </c>
+      <c r="B227" t="s">
+        <v>75</v>
+      </c>
+      <c r="C227">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
+        <v>82</v>
+      </c>
+      <c r="B228" t="s">
+        <v>76</v>
+      </c>
+      <c r="C228">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A229" t="s">
+        <v>82</v>
+      </c>
+      <c r="B229" t="s">
+        <v>77</v>
+      </c>
+      <c r="C229">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
+        <v>82</v>
+      </c>
+      <c r="B230" t="s">
+        <v>78</v>
+      </c>
+      <c r="C230">
+        <v>2.3</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
+        <v>82</v>
+      </c>
+      <c r="B231" t="s">
+        <v>79</v>
+      </c>
+      <c r="C231">
+        <v>2.2</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>82</v>
+      </c>
+      <c r="B232" t="s">
         <v>80</v>
       </c>
-      <c r="B226" t="s">
-        <v>78</v>
-      </c>
-      <c r="C226">
-        <v>2.3</v>
+      <c r="C232">
+        <v>3.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
UPD data from 2020-05-12
</commit_message>
<xml_diff>
--- a/index_si_moscow_stpetersburg_sevastopol.xlsx
+++ b/index_si_moscow_stpetersburg_sevastopol.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="85">
   <si>
     <t>state</t>
   </si>
@@ -254,6 +254,12 @@
   </si>
   <si>
     <t>2020-05-09</t>
+  </si>
+  <si>
+    <t>2020-05-10</t>
+  </si>
+  <si>
+    <t>2020-05-11</t>
   </si>
   <si>
     <t>Севастополь</t>
@@ -639,7 +645,7 @@
   <sheetPr>
     <tabColor rgb="FFEBA00"/>
   </sheetPr>
-  <dimension ref="A1:C232"/>
+  <dimension ref="A1:C238"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
@@ -1506,54 +1512,54 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
+        <v>3</v>
+      </c>
+      <c r="B79" t="s">
         <v>81</v>
       </c>
-      <c r="B79" t="s">
-        <v>4</v>
-      </c>
       <c r="C79">
-        <v>3</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>81</v>
+        <v>3</v>
       </c>
       <c r="B80" t="s">
-        <v>5</v>
+        <v>82</v>
       </c>
       <c r="C80">
-        <v>3.4</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B81" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C81">
-        <v>1.6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B82" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C82">
-        <v>1.6</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B83" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C83">
         <v>1.6</v>
@@ -1561,87 +1567,87 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C84">
-        <v>1.7</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B85" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C85">
-        <v>2.6</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B86" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C86">
-        <v>3</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B87" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C87">
-        <v>1.7</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B88" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C88">
-        <v>1.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B89" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C89">
-        <v>1.4</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B90" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C90">
-        <v>1.4</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B91" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C91">
         <v>1.4</v>
@@ -1649,318 +1655,318 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B92" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C92">
-        <v>2.3</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B93" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C93">
-        <v>2.6</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B94" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C94">
-        <v>2.9</v>
+        <v>2.3</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B95" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C95">
-        <v>1.5</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B96" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C96">
-        <v>1.5</v>
+        <v>2.9</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B97" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C97">
-        <v>1.4</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B98" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C98">
-        <v>1.4</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B99" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C99">
-        <v>2.5</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B100" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C100">
-        <v>3.3</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B101" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C101">
-        <v>1.6</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B102" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C102">
-        <v>1.5</v>
+        <v>3.3</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B103" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C103">
-        <v>2.5</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B104" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C104">
-        <v>1.9</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B105" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C105">
-        <v>1.8</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B106" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C106">
-        <v>2.5</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B107" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C107">
-        <v>3.1</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B108" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C108">
-        <v>2.1</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B109" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C109">
-        <v>2</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B110" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C110">
-        <v>1.9</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B111" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C111">
-        <v>1.9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B112" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C112">
-        <v>2</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B113" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C113">
-        <v>3.1</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B114" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C114">
-        <v>3.7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B115" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C115">
-        <v>3.2</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B116" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C116">
-        <v>3.4</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B117" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C117">
-        <v>3.6</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B118" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C118">
-        <v>3.9</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B119" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C119">
-        <v>3.7</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B120" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C120">
         <v>3.9</v>
@@ -1968,175 +1974,175 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B121" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C121">
-        <v>4.1</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B122" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C122">
-        <v>3.5</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B123" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C123">
-        <v>3.4</v>
+        <v>4.1</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B124" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C124">
-        <v>3.3</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B125" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C125">
-        <v>3.3</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B126" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C126">
-        <v>3.2</v>
+        <v>3.3</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B127" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C127">
-        <v>3.5</v>
+        <v>3.3</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B128" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C128">
-        <v>3.9</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B129" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C129">
-        <v>3.2</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B130" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C130">
-        <v>3.1</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B131" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C131">
-        <v>3.3</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B132" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C132">
-        <v>3.2</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B133" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C133">
-        <v>3.1</v>
+        <v>3.3</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B134" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C134">
-        <v>3.5</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B135" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C135">
-        <v>3.8</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B136" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C136">
         <v>3.5</v>
@@ -2144,32 +2150,32 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B137" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C137">
-        <v>3</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B138" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C138">
-        <v>3</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B139" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C139">
         <v>3</v>
@@ -2177,120 +2183,120 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B140" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C140">
-        <v>2.9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B141" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C141">
-        <v>3.3</v>
+        <v>3</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B142" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C142">
-        <v>3.8</v>
+        <v>2.9</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B143" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C143">
-        <v>2.9</v>
+        <v>3.3</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B144" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C144">
-        <v>2.8</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B145" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C145">
-        <v>2.8</v>
+        <v>2.9</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B146" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C146">
-        <v>2.7</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B147" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C147">
-        <v>3.2</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B148" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C148">
-        <v>3.3</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B149" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C149">
-        <v>3.5</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B150" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C150">
         <v>3.3</v>
@@ -2298,241 +2304,241 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B151" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C151">
-        <v>3.2</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B152" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C152">
-        <v>2.7</v>
+        <v>3.3</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B153" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C153">
-        <v>2.7</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B154" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C154">
-        <v>2.8</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B155" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C155">
-        <v>3.3</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B156" t="s">
-        <v>4</v>
+        <v>79</v>
       </c>
       <c r="C156">
-        <v>2.5</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B157" t="s">
-        <v>5</v>
+        <v>80</v>
       </c>
       <c r="C157">
-        <v>2.6</v>
+        <v>3.3</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B158" t="s">
-        <v>6</v>
+        <v>81</v>
       </c>
       <c r="C158">
-        <v>0.4</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
+        <v>83</v>
+      </c>
+      <c r="B159" t="s">
         <v>82</v>
       </c>
-      <c r="B159" t="s">
-        <v>7</v>
-      </c>
       <c r="C159">
-        <v>0.4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B160" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C160">
-        <v>0.4</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B161" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C161">
-        <v>0.5</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B162" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C162">
-        <v>2</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B163" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C163">
-        <v>2.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B164" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C164">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B165" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C165">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B166" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C166">
-        <v>0.4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B167" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C167">
-        <v>0.4</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B168" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C168">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B169" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C169">
-        <v>2</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B170" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C170">
-        <v>2.4</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B171" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C171">
-        <v>2.4</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B172" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C172">
         <v>0.4</v>
@@ -2540,384 +2546,384 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B173" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C173">
-        <v>0.4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B174" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C174">
-        <v>0.5</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B175" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C175">
-        <v>0.5</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B176" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C176">
-        <v>2.1</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B177" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C177">
-        <v>2.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B178" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C178">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B179" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C179">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B180" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C180">
-        <v>0.8</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B181" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C181">
-        <v>0.9</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B182" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C182">
-        <v>0.9</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B183" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C183">
-        <v>2.4</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B184" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C184">
-        <v>2.8</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B185" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C185">
-        <v>1</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B186" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C186">
-        <v>1.1</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B187" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C187">
-        <v>1</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B188" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C188">
-        <v>1.1</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B189" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C189">
-        <v>1.1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B190" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C190">
-        <v>3</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B191" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C191">
-        <v>3.6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B192" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C192">
-        <v>3</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B193" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C193">
-        <v>3.2</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B194" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C194">
-        <v>3.4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B195" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C195">
-        <v>3.5</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B196" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C196">
-        <v>3.4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B197" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C197">
-        <v>3.8</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B198" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C198">
-        <v>3.9</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B199" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C199">
-        <v>2.9</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B200" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C200">
-        <v>2.8</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B201" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C201">
-        <v>2.8</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B202" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C202">
-        <v>2.8</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B203" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C203">
-        <v>2.7</v>
+        <v>2.9</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B204" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C204">
-        <v>3.5</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B205" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C205">
-        <v>3.8</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B206" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C206">
-        <v>2.7</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B207" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C207">
         <v>2.7</v>
@@ -2925,32 +2931,32 @@
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B208" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C208">
-        <v>2.7</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B209" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C209">
-        <v>2.7</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B210" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C210">
         <v>2.7</v>
@@ -2958,32 +2964,32 @@
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B211" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C211">
-        <v>3.5</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B212" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C212">
-        <v>3.8</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B213" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C213">
         <v>2.7</v>
@@ -2991,76 +2997,76 @@
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B214" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C214">
-        <v>2.6</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B215" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C215">
-        <v>2.6</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B216" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C216">
-        <v>2.5</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B217" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C217">
-        <v>2.6</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B218" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C218">
-        <v>3.2</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B219" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C219">
-        <v>3.6</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B220" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C220">
         <v>2.5</v>
@@ -3068,134 +3074,200 @@
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B221" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C221">
-        <v>2.4</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B222" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C222">
-        <v>2.4</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B223" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C223">
-        <v>2.3</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B224" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C224">
-        <v>3.1</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B225" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C225">
-        <v>3.1</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B226" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C226">
-        <v>3.4</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B227" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C227">
-        <v>3</v>
+        <v>2.3</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B228" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C228">
-        <v>2.9</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B229" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C229">
-        <v>2.1</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B230" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C230">
-        <v>2.3</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B231" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C231">
-        <v>2.2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
+        <v>84</v>
+      </c>
+      <c r="B232" t="s">
+        <v>76</v>
+      </c>
+      <c r="C232">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
+        <v>84</v>
+      </c>
+      <c r="B233" t="s">
+        <v>77</v>
+      </c>
+      <c r="C233">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
+        <v>84</v>
+      </c>
+      <c r="B234" t="s">
+        <v>78</v>
+      </c>
+      <c r="C234">
+        <v>2.3</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
+        <v>84</v>
+      </c>
+      <c r="B235" t="s">
+        <v>79</v>
+      </c>
+      <c r="C235">
+        <v>2.2</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
+        <v>84</v>
+      </c>
+      <c r="B236" t="s">
+        <v>80</v>
+      </c>
+      <c r="C236">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
+        <v>84</v>
+      </c>
+      <c r="B237" t="s">
+        <v>81</v>
+      </c>
+      <c r="C237">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
+        <v>84</v>
+      </c>
+      <c r="B238" t="s">
         <v>82</v>
       </c>
-      <c r="B232" t="s">
-        <v>80</v>
-      </c>
-      <c r="C232">
-        <v>3.1</v>
+      <c r="C238">
+        <v>2.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>